<commit_message>
Updated the evaluation notes and order
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anders S. Johansen\Documents\MED10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{350CDF53-3DE3-4174-9AAA-9A60651BDE5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BD79EB-CF4F-4C7B-8354-900812DBAFA0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2136" yWindow="0" windowWidth="19056" windowHeight="9276" activeTab="1" xr2:uid="{36F197DF-833F-4971-8683-502A5D50ECB2}"/>
+    <workbookView xWindow="-8256" yWindow="3084" windowWidth="19056" windowHeight="9276" activeTab="1" xr2:uid="{36F197DF-833F-4971-8683-502A5D50ECB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
   <si>
     <t>Participant 1</t>
   </si>
@@ -134,6 +134,33 @@
   </si>
   <si>
     <t xml:space="preserve">D A B C </t>
+  </si>
+  <si>
+    <t>participant 1</t>
+  </si>
+  <si>
+    <t>participant 2</t>
+  </si>
+  <si>
+    <t>participant 3</t>
+  </si>
+  <si>
+    <t>A B C</t>
+  </si>
+  <si>
+    <t>B C A</t>
+  </si>
+  <si>
+    <t>C A B</t>
+  </si>
+  <si>
+    <t>A = SLOW</t>
+  </si>
+  <si>
+    <t>B =MEDIUM</t>
+  </si>
+  <si>
+    <t>C = FAST</t>
   </si>
 </sst>
 </file>
@@ -157,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -165,12 +192,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,10 +743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565192FC-457A-45E0-B26D-E6CA912763DD}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C28" sqref="A26:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,7 +758,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D1" t="s">
@@ -702,7 +769,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
@@ -713,18 +780,18 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
@@ -735,7 +802,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -743,7 +810,7 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -751,15 +818,15 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -767,7 +834,7 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -775,7 +842,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -783,50 +850,122 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>